<commit_message>
add file exel db
</commit_message>
<xml_diff>
--- a/Diagram and flowchart/dbDesign.xlsx
+++ b/Diagram and flowchart/dbDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\datn-j2teamnnl\Diagram and flowchart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41A1A9F4-6DED-4B16-A04E-CA2245F6AEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2FE7F2-3C26-4F42-95B6-B388E538E140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F3F8D47C-8E8D-435C-A43D-11D0DA7C41EE}"/>
   </bookViews>
@@ -31,6 +31,137 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>subAdmin</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>describe</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdt </t>
+  </si>
+  <si>
+    <t>ghi chu</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>totalCost</t>
+  </si>
+  <si>
+    <t>payment</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>shipment</t>
+  </si>
+  <si>
+    <t>SDTime</t>
+  </si>
+  <si>
+    <t>DVtime</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>paymentType</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -42,12 +173,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,8 +199,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,12 +516,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9441F0-4B14-4099-9A59-B29B7B26A484}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
diagram and flowchar add a new img descibe entity realtionship database
</commit_message>
<xml_diff>
--- a/Diagram and flowchart/dbDesign.xlsx
+++ b/Diagram and flowchart/dbDesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\datn-j2teamnnl\Diagram and flowchart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2FE7F2-3C26-4F42-95B6-B388E538E140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817CB8BA-E1B6-4ECE-8645-091F2446F22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F3F8D47C-8E8D-435C-A43D-11D0DA7C41EE}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>admin</t>
   </si>
@@ -94,18 +94,9 @@
     <t>ten</t>
   </si>
   <si>
-    <t xml:space="preserve">sdt </t>
-  </si>
-  <si>
-    <t>ghi chu</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
-    <t>heading</t>
-  </si>
-  <si>
     <t>content</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>payment</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -158,6 +146,9 @@
   </si>
   <si>
     <t>paymentType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -516,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9441F0-4B14-4099-9A59-B29B7B26A484}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -583,12 +574,12 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -614,19 +605,19 @@
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -657,19 +648,19 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O12" t="s">
         <v>17</v>
@@ -683,16 +674,13 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
         <v>32</v>
       </c>
-      <c r="M13" t="s">
-        <v>36</v>
-      </c>
       <c r="O13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -702,11 +690,8 @@
       <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
       <c r="O14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -714,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="O15" t="s">
         <v>8</v>
@@ -725,20 +710,20 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="O16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>17</v>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>